<commit_message>
Repaired MSV, now it glows even in night. Repaired bogies.
</commit_message>
<xml_diff>
--- a/Source/Smejki/CD460pack01/RailVehicles/Electric/Common/Script/460_TCHedb.xlsx
+++ b/Source/Smejki/CD460pack01/RailVehicles/Electric/Common/Script/460_TCHedb.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Games\Train Simulator 2017\Source\CS_addon\Smejki\RailVehicles\Electric\460080\EngineScr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Games\Train Simulator 2017\Source\Smejki\CD460pack01\RailVehicles\Electric\Common\Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -361,11 +361,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="216292992"/>
-        <c:axId val="216293552"/>
+        <c:axId val="306216816"/>
+        <c:axId val="306217376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="216292992"/>
+        <c:axId val="306216816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -408,7 +408,7 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216293552"/>
+        <c:crossAx val="306217376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -416,7 +416,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216293552"/>
+        <c:axId val="306217376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -467,7 +467,7 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216292992"/>
+        <c:crossAx val="306216816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -777,11 +777,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="295443504"/>
-        <c:axId val="295444064"/>
+        <c:axId val="306221296"/>
+        <c:axId val="306221856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="295443504"/>
+        <c:axId val="306221296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -824,7 +824,7 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="295444064"/>
+        <c:crossAx val="306221856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -832,7 +832,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="295444064"/>
+        <c:axId val="306221856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -883,7 +883,7 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="295443504"/>
+        <c:crossAx val="306221296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -897,7 +897,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2414,7 +2413,7 @@
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2495,7 +2494,7 @@
         <v>20.723404255319149</v>
       </c>
       <c r="H2">
-        <f t="shared" si="0"/>
+        <f>($N$9+($N$8*H3))/(($N$10*H3)+$N$11)+$P$8</f>
         <v>21.23076923076923</v>
       </c>
       <c r="I2">

</xml_diff>